<commit_message>
Estado del arte mejorado
</commit_message>
<xml_diff>
--- a/command.xlsx
+++ b/command.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcarsala/Examen-de-Calificacion-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA73578B-9825-5C42-BFE4-98B254B17425}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55CD61-95A3-F34A-9901-8F651D2F713E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7D077E3C-DE8E-154E-8E31-7F2103695097}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparsion AV1 vs HEVC" sheetId="1" r:id="rId1"/>
     <sheet name="Bibliography review" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Intra</t>
   </si>
@@ -111,16 +112,411 @@
   </si>
   <si>
     <t>﻿Dong, L. I. U., Yue, L. I., Jianping, L. I. N., Houqiang, L. I., &amp; Feng, W. U. (2020). Deep learning-based video coding: A review and a case study. In ACM Computing Surveys (Vol. 53, Issue 1). https://doi.org/10.1145/3368405</t>
+  </si>
+  <si>
+    <t>Deep Tool /Deep Coding</t>
+  </si>
+  <si>
+    <t>H.264</t>
+  </si>
+  <si>
+    <t>HEVC</t>
+  </si>
+  <si>
+    <t>MPEG-2</t>
+  </si>
+  <si>
+    <t>VP9</t>
+  </si>
+  <si>
+    <t>AV1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Panayides, A. S., Pattichis, M. S., Pantziaris, M., Constantinides, A. G., &amp; Pattichis, C. S. (2020). The Battle of the Video Codecs in the Healthcare Domain - A Comparative Performance Evaluation Study Leveraging VVC and AV1. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IEEE Access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 11469–11481. https://doi.org/10.1109/ACCESS.2020.2965325</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bitmovin. (2019). Video Developer Report 2019. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bitmovin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 80. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sandvine, (2020). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phenomena Report COVID-19 Spotlight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sandvine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bross, Benjamin, JIANLE CHEN, JENS-RAINER OHM, GARY J. SULLIVAN, Y.-K. W. (2020). Developments in International Video Coding Standardization After AVC with an Overview of Versatile Video Coding. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proc_IEEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>July</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 1–31. https://doi.org/10.1109/JPROC.2020.3043399</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lei, R., Zhao, X., Ronca, D., Choi, K., Katsavounidis, I., Xu, Y., &amp; Krishnan, J. (2020). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AOM Video Codec Requirements Draft Proposal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Karwowski, D., Grajek, T., Klimaszewski, K., Stankiewicz, O., Stankowski, J., &amp; Wegner, K. (2017). 20 years of progress in video compression – From MPEG-1 to MPEG-H HEVC. General view on the path of video coding development. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Advances in Intelligent Systems and Computing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>525</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(October), 3–15. https://doi.org/10.1007/978-3-319-47274-4_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Birman, R., Segal, Y., &amp; Hadar, O. (2020). Overview of Research in the field of Video Compression using Deep Neural Networks. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multimedia Tools and Applications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(17–18), 11699–11722. https://doi.org/10.1007/s11042-019-08572-3</t>
+    </r>
+  </si>
+  <si>
+    <t>Restoration filters</t>
+  </si>
+  <si>
+    <t>Video codec adoption</t>
+  </si>
+  <si>
+    <t>Global internet traffic</t>
+  </si>
+  <si>
+    <t>VVC</t>
+  </si>
+  <si>
+    <t>AV2</t>
+  </si>
+  <si>
+    <t>History of video coding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -156,6 +552,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -172,6 +572,1025 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CO"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$3:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>H.264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>HEVC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPEG-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VP9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AV1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7505-CC47-8219-746625C97404}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8B366F0-7254-2F40-BE5F-B65B894D2094}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D8AAFA-EF33-344A-8900-E989E436B4AB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,8 +2140,141 @@
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD4A57D-1EFF-7E45-81A8-1C391DF897EB}">
+  <dimension ref="B3:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>91</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Respuestas para el profesor Germán
</commit_message>
<xml_diff>
--- a/command.xlsx
+++ b/command.xlsx
@@ -8,15 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcarsala/Examen-de-Calificacion-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55CD61-95A3-F34A-9901-8F651D2F713E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A871054-CFDC-0C48-BFB2-5CA3702812AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7D077E3C-DE8E-154E-8E31-7F2103695097}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21060" xr2:uid="{7D077E3C-DE8E-154E-8E31-7F2103695097}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparsion AV1 vs HEVC" sheetId="1" r:id="rId1"/>
     <sheet name="Bibliography review" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Comparsion AV1 vs HEVC'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Comparsion AV1 vs HEVC'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Comparsion AV1 vs HEVC'!#REF!</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Comparsion AV1 vs HEVC'!$D$2:$E$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -28,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Intra</t>
   </si>
@@ -36,12 +74,6 @@
     <t>Medeley</t>
   </si>
   <si>
-    <t>Search patron</t>
-  </si>
-  <si>
-    <t>Intra+prediction+hevc</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -51,52 +83,7 @@
     <t>2018-2021</t>
   </si>
   <si>
-    <t>Intra+prediction+av1</t>
-  </si>
-  <si>
-    <t>Inter+prediction+av1</t>
-  </si>
-  <si>
-    <t>Inter+prediction+hevc</t>
-  </si>
-  <si>
     <t>Scopus</t>
-  </si>
-  <si>
-    <t>transform+hevc</t>
-  </si>
-  <si>
-    <t>transform+av1</t>
-  </si>
-  <si>
-    <t>quantization+hevc</t>
-  </si>
-  <si>
-    <t>quantization+av1</t>
-  </si>
-  <si>
-    <t>entropy+av1</t>
-  </si>
-  <si>
-    <t>entropy+hevc</t>
-  </si>
-  <si>
-    <t>restoration+hevc</t>
-  </si>
-  <si>
-    <t>restoration+av1</t>
-  </si>
-  <si>
-    <t>deep+hevc</t>
-  </si>
-  <si>
-    <t>deep+av1</t>
-  </si>
-  <si>
-    <t>Total ML based tools in HEVC</t>
-  </si>
-  <si>
-    <t>Total ML based tools in aV1</t>
   </si>
   <si>
     <t>Name</t>
@@ -485,12 +472,36 @@
   <si>
     <t>History of video coding</t>
   </si>
+  <si>
+    <t>Transform</t>
+  </si>
+  <si>
+    <t>Quantization</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Restoration</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>Inter prediction</t>
+  </si>
+  <si>
+    <t>Intra prediction</t>
+  </si>
+  <si>
+    <t>DL+video coding</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -521,16 +532,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -538,25 +563,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,6 +624,463 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$E$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HEVC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="89000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="23000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="89000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="69000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="97000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="70000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+              </a:path>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$D$24:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Intra prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Inter prediction</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Transform</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quantization</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Entropy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Restoration</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DL+video coding</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$E$24:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4D17-B143-AB8D-D60F00930B92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AV1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="46000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="130000" r="50000" b="-30000"/>
+              </a:path>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$D$24:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Intra prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Inter prediction</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Transform</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quantization</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Entropy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Restoration</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DL+video coding</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparsion AV1 vs HEVC'!$F$24:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4D17-B143-AB8D-D60F00930B92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1227786287"/>
+        <c:axId val="1291021919"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1227786287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1291021919"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1291021919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1227786287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1050,36 +1556,74 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1087,37 +1631,44 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1136,14 +1687,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1157,7 +1700,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -1167,7 +1710,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -1177,7 +1720,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -1197,7 +1740,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -1216,6 +1759,505 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -1553,6 +2595,47 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>741475</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>192424</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>69529</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A10357BA-4069-BC41-9BEF-2C5C2DC22AD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1890,219 +2973,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3070C4DC-1DE7-0941-92E7-3AC8F07BB521}">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
         <v>426</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>308</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
+      <c r="H2">
+        <f>ROUND(AVERAGE(F2,G2),0)</f>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D3" s="9"/>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+      <c r="H3">
+        <f t="shared" ref="H3:H15" si="0">ROUND(AVERAGE(F3,G3),0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>610</v>
+      </c>
+      <c r="G4">
+        <v>165</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E4">
-        <v>610</v>
-      </c>
-      <c r="F4">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>284</v>
+      </c>
+      <c r="G6">
+        <v>214</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="9"/>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+      <c r="G7">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="H7">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>284</v>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
       <c r="F8">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>14</v>
+        <v>240</v>
+      </c>
+      <c r="G8">
+        <v>166</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="9"/>
+      <c r="E9" t="s">
+        <v>16</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="E11">
-        <v>240</v>
+      <c r="F10">
+        <v>261</v>
+      </c>
+      <c r="G10">
+        <v>63</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D11" s="9"/>
+      <c r="E11" t="s">
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12">
         <v>8</v>
       </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
       <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D13" s="9"/>
+      <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="E14">
-        <v>261</v>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14">
+        <v>104</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="9"/>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <v>367</v>
+      </c>
+      <c r="F24">
         <v>15</v>
       </c>
-      <c r="E15">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17">
-        <v>12</v>
-      </c>
-      <c r="F17">
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25">
+        <v>388</v>
+      </c>
+      <c r="F25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>249</v>
+      </c>
+      <c r="F26">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>203</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>162</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
+      </c>
+      <c r="F29" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20">
-        <v>200</v>
-      </c>
-      <c r="F20">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30">
+        <v>152</v>
+      </c>
+      <c r="F30">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2110,8 +3349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D8AAFA-EF33-344A-8900-E989E436B4AB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2121,83 +3360,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2220,7 +3459,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>91</v>
@@ -2231,7 +3470,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>43</v>
@@ -2242,7 +3481,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>29</v>
@@ -2253,9 +3492,9 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
         <v>11</v>
       </c>
       <c r="D6">
@@ -2264,7 +3503,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>7</v>

</xml_diff>